<commit_message>
config demais routers e sw
</commit_message>
<xml_diff>
--- a/Cálculo Endereçamento IP - T1 e T2 - Ciclo 11 - 05-12-2025.xlsx
+++ b/Cálculo Endereçamento IP - T1 e T2 - Ciclo 11 - 05-12-2025.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rodri\OneDrive\Documentos\LAB ONDA 11\REDE-SP-RJ\LAB-REDE-SP-RJ\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A45A9D8-3E64-4982-917A-7E34367C834D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CD49F86-AD43-4CA2-A229-346D8A1D6C9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{C9898CB8-8B09-4813-8ED8-B3EC6FFD7678}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="639" uniqueCount="419">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="640" uniqueCount="420">
   <si>
     <r>
       <t>2^</t>
@@ -3896,6 +3896,9 @@
   </si>
   <si>
     <t>192.168.1.27</t>
+  </si>
+  <si>
+    <t>172.23.0.0</t>
   </si>
 </sst>
 </file>
@@ -4955,12 +4958,156 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="6" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="6" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="6" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="6" fillId="5" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="6" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="29" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="29" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="29" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="29" fillId="5" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -4976,149 +5123,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="6" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="6" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="6" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="6" fillId="5" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="6" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="29" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="29" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="29" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="29" fillId="5" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="12" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="15" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="17" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -5149,24 +5170,6 @@
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="2" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="2" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="2" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="12" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="15" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="17" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -5535,7 +5538,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E17E603A-89D7-4345-879A-C03052B99BF9}">
   <dimension ref="A1:I26"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView topLeftCell="A2" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
@@ -5754,7 +5757,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B143EED-3CFE-47B8-B44E-4CD1617A7E15}">
   <dimension ref="A1:AF156"/>
   <sheetViews>
-    <sheetView topLeftCell="O1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView topLeftCell="L1" zoomScale="88" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="T5" sqref="T5"/>
     </sheetView>
   </sheetViews>
@@ -5770,20 +5773,24 @@
     <col min="9" max="9" width="8.90625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="9.453125" customWidth="1"/>
     <col min="13" max="13" width="4.81640625" customWidth="1"/>
+    <col min="15" max="15" width="8.81640625" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="12.1796875" customWidth="1"/>
     <col min="19" max="19" width="10.54296875" customWidth="1"/>
+    <col min="20" max="20" width="8.81640625" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="14.08984375" customWidth="1"/>
-    <col min="25" max="25" width="15.1796875" bestFit="1" customWidth="1"/>
-    <col min="26" max="27" width="11.453125" bestFit="1" customWidth="1"/>
+    <col min="22" max="24" width="8.81640625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="15.26953125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="12.1796875" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="13.6328125" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="27.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:32" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="156" t="s">
+      <c r="A1" s="187" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="156" t="s">
+      <c r="B1" s="187" t="s">
         <v>17</v>
       </c>
       <c r="C1" s="13" t="s">
@@ -5813,8 +5820,8 @@
       <c r="Z1" s="148"/>
     </row>
     <row r="2" spans="1:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="157"/>
-      <c r="B2" s="157"/>
+      <c r="A2" s="188"/>
+      <c r="B2" s="188"/>
       <c r="C2" s="14" t="s">
         <v>19</v>
       </c>
@@ -6287,11 +6294,11 @@
       <c r="S10" s="10"/>
       <c r="U10" s="10"/>
       <c r="V10" s="10"/>
-      <c r="Y10" s="158" t="s">
+      <c r="Y10" s="189" t="s">
         <v>293</v>
       </c>
-      <c r="Z10" s="158"/>
-      <c r="AA10" s="158"/>
+      <c r="Z10" s="189"/>
+      <c r="AA10" s="189"/>
     </row>
     <row r="11" spans="1:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A11" s="20">
@@ -6389,7 +6396,7 @@
       <c r="C15" s="25">
         <v>0</v>
       </c>
-      <c r="D15" s="160"/>
+      <c r="D15" s="193"/>
       <c r="H15" t="s">
         <v>88</v>
       </c>
@@ -6416,7 +6423,7 @@
       <c r="C16" s="33" t="s">
         <v>53</v>
       </c>
-      <c r="D16" s="161"/>
+      <c r="D16" s="194"/>
       <c r="G16" t="s">
         <v>85</v>
       </c>
@@ -6448,7 +6455,7 @@
       <c r="C17" s="29">
         <v>0</v>
       </c>
-      <c r="D17" s="162" t="s">
+      <c r="D17" s="195" t="s">
         <v>43</v>
       </c>
       <c r="H17">
@@ -6480,7 +6487,7 @@
       <c r="C18" s="34" t="s">
         <v>53</v>
       </c>
-      <c r="D18" s="163"/>
+      <c r="D18" s="196"/>
       <c r="H18">
         <v>1</v>
       </c>
@@ -6506,7 +6513,7 @@
       <c r="C19" s="32">
         <v>1</v>
       </c>
-      <c r="D19" s="164" t="s">
+      <c r="D19" s="197" t="s">
         <v>46</v>
       </c>
       <c r="H19">
@@ -6541,14 +6548,14 @@
       <c r="C20" s="33" t="s">
         <v>54</v>
       </c>
-      <c r="D20" s="165"/>
+      <c r="D20" s="198"/>
       <c r="M20" s="6">
         <v>255255255192</v>
       </c>
-      <c r="R20" s="149" t="s">
+      <c r="R20" s="190" t="s">
         <v>346</v>
       </c>
-      <c r="S20" s="150"/>
+      <c r="S20" s="191"/>
       <c r="U20" s="75"/>
       <c r="V20" s="76"/>
       <c r="Y20" s="71" t="s">
@@ -6568,7 +6575,7 @@
       <c r="C21" s="29">
         <v>254</v>
       </c>
-      <c r="D21" s="162" t="s">
+      <c r="D21" s="195" t="s">
         <v>49</v>
       </c>
       <c r="H21" t="s">
@@ -6600,7 +6607,7 @@
       <c r="C22" s="30">
         <v>11111110</v>
       </c>
-      <c r="D22" s="163"/>
+      <c r="D22" s="196"/>
       <c r="H22">
         <v>1</v>
       </c>
@@ -6649,7 +6656,7 @@
       <c r="C23" s="32">
         <v>255</v>
       </c>
-      <c r="D23" s="164" t="s">
+      <c r="D23" s="197" t="s">
         <v>52</v>
       </c>
       <c r="H23">
@@ -6683,7 +6690,7 @@
       <c r="C24" s="26">
         <v>11111111</v>
       </c>
-      <c r="D24" s="165"/>
+      <c r="D24" s="198"/>
       <c r="H24">
         <v>1</v>
       </c>
@@ -6700,10 +6707,10 @@
       <c r="V24" s="74"/>
       <c r="Y24" s="84"/>
       <c r="Z24" s="85"/>
-      <c r="AA24" s="151" t="s">
+      <c r="AA24" s="199" t="s">
         <v>284</v>
       </c>
-      <c r="AB24" s="152"/>
+      <c r="AB24" s="200"/>
     </row>
     <row r="25" spans="1:31" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="H25">
@@ -6747,10 +6754,10 @@
       </c>
       <c r="U26" s="73"/>
       <c r="V26" s="74"/>
-      <c r="Y26" s="153" t="s">
+      <c r="Y26" s="201" t="s">
         <v>269</v>
       </c>
-      <c r="Z26" s="154"/>
+      <c r="Z26" s="202"/>
       <c r="AA26" s="82" t="s">
         <v>281</v>
       </c>
@@ -6831,10 +6838,10 @@
         <v>282</v>
       </c>
       <c r="Z29" s="81"/>
-      <c r="AA29" s="151" t="s">
+      <c r="AA29" s="199" t="s">
         <v>287</v>
       </c>
-      <c r="AB29" s="152"/>
+      <c r="AB29" s="200"/>
     </row>
     <row r="30" spans="1:31" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="R30" s="71" t="s">
@@ -6875,10 +6882,10 @@
       <c r="AB31" s="74"/>
     </row>
     <row r="32" spans="1:31" x14ac:dyDescent="0.35">
-      <c r="A32" s="159" t="s">
+      <c r="A32" s="192" t="s">
         <v>65</v>
       </c>
-      <c r="B32" s="159"/>
+      <c r="B32" s="192"/>
       <c r="R32" s="73" t="s">
         <v>357</v>
       </c>
@@ -6933,10 +6940,10 @@
       </c>
       <c r="U34" s="73"/>
       <c r="V34" s="74"/>
-      <c r="AA34" s="155" t="s">
+      <c r="AA34" s="203" t="s">
         <v>300</v>
       </c>
-      <c r="AB34" s="152"/>
+      <c r="AB34" s="200"/>
     </row>
     <row r="35" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A35" s="39" t="s">
@@ -7041,8 +7048,8 @@
       <c r="S41" s="74" t="s">
         <v>258</v>
       </c>
-      <c r="U41" s="155"/>
-      <c r="V41" s="152"/>
+      <c r="U41" s="203"/>
+      <c r="V41" s="200"/>
     </row>
     <row r="42" spans="1:28" x14ac:dyDescent="0.35">
       <c r="R42" s="73" t="s">
@@ -7205,16 +7212,16 @@
       </c>
     </row>
     <row r="55" spans="1:26" ht="16" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A55" s="170" t="s">
+      <c r="A55" s="184" t="s">
         <v>21</v>
       </c>
-      <c r="B55" s="170" t="s">
+      <c r="B55" s="184" t="s">
         <v>79</v>
       </c>
       <c r="C55" s="40" t="s">
         <v>80</v>
       </c>
-      <c r="D55" s="171">
+      <c r="D55" s="164">
         <v>16777214</v>
       </c>
       <c r="R55" s="75" t="s">
@@ -7231,32 +7238,32 @@
       <c r="Z55" s="148"/>
     </row>
     <row r="56" spans="1:26" ht="15.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A56" s="167"/>
-      <c r="B56" s="167"/>
+      <c r="A56" s="183"/>
+      <c r="B56" s="183"/>
       <c r="C56" s="41">
         <v>1.1111111E+31</v>
       </c>
-      <c r="D56" s="172"/>
-      <c r="R56" s="149" t="s">
+      <c r="D56" s="152"/>
+      <c r="R56" s="190" t="s">
         <v>296</v>
       </c>
-      <c r="S56" s="150"/>
+      <c r="S56" s="191"/>
       <c r="U56" s="71"/>
       <c r="V56" s="72"/>
       <c r="Y56" s="71"/>
       <c r="Z56" s="72"/>
     </row>
     <row r="57" spans="1:26" ht="15" x14ac:dyDescent="0.35">
-      <c r="A57" s="173" t="s">
+      <c r="A57" s="185" t="s">
         <v>23</v>
       </c>
-      <c r="B57" s="173" t="s">
+      <c r="B57" s="185" t="s">
         <v>81</v>
       </c>
       <c r="C57" s="42" t="s">
         <v>82</v>
       </c>
-      <c r="D57" s="175">
+      <c r="D57" s="157">
         <v>65534</v>
       </c>
       <c r="R57" s="71" t="s">
@@ -7271,12 +7278,12 @@
       <c r="Z57" s="74"/>
     </row>
     <row r="58" spans="1:26" ht="15.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A58" s="174"/>
-      <c r="B58" s="174"/>
+      <c r="A58" s="186"/>
+      <c r="B58" s="186"/>
       <c r="C58" s="43">
         <v>1.1111111111111101E+31</v>
       </c>
-      <c r="D58" s="176"/>
+      <c r="D58" s="158"/>
       <c r="R58" s="73" t="s">
         <v>382</v>
       </c>
@@ -7289,16 +7296,16 @@
       <c r="Z58" s="76"/>
     </row>
     <row r="59" spans="1:26" ht="15.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A59" s="166" t="s">
+      <c r="A59" s="182" t="s">
         <v>25</v>
       </c>
-      <c r="B59" s="166" t="s">
+      <c r="B59" s="182" t="s">
         <v>83</v>
       </c>
       <c r="C59" s="44" t="s">
         <v>84</v>
       </c>
-      <c r="D59" s="168">
+      <c r="D59" s="149">
         <v>254</v>
       </c>
       <c r="R59" s="73" t="s">
@@ -7315,12 +7322,12 @@
       <c r="Z59" s="148"/>
     </row>
     <row r="60" spans="1:26" ht="15.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A60" s="167"/>
-      <c r="B60" s="167"/>
+      <c r="A60" s="183"/>
+      <c r="B60" s="183"/>
       <c r="C60" s="41">
         <v>1.1111111111111101E+31</v>
       </c>
-      <c r="D60" s="169"/>
+      <c r="D60" s="150"/>
       <c r="R60" s="73" t="s">
         <v>384</v>
       </c>
@@ -7392,19 +7399,19 @@
       <c r="Z64" s="72"/>
     </row>
     <row r="65" spans="1:26" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A65" s="200" t="s">
+      <c r="A65" s="161" t="s">
         <v>76</v>
       </c>
-      <c r="B65" s="200" t="s">
+      <c r="B65" s="161" t="s">
         <v>35</v>
       </c>
       <c r="C65" s="46" t="s">
         <v>209</v>
       </c>
-      <c r="D65" s="200" t="s">
+      <c r="D65" s="161" t="s">
         <v>211</v>
       </c>
-      <c r="E65" s="200" t="s">
+      <c r="E65" s="161" t="s">
         <v>78</v>
       </c>
       <c r="R65" s="146" t="s">
@@ -7417,13 +7424,13 @@
       <c r="Z65" s="74"/>
     </row>
     <row r="66" spans="1:26" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A66" s="201"/>
-      <c r="B66" s="201"/>
+      <c r="A66" s="162"/>
+      <c r="B66" s="162"/>
       <c r="C66" s="52" t="s">
         <v>210</v>
       </c>
-      <c r="D66" s="201"/>
-      <c r="E66" s="201"/>
+      <c r="D66" s="162"/>
+      <c r="E66" s="162"/>
       <c r="R66" s="71" t="s">
         <v>355</v>
       </c>
@@ -7436,19 +7443,19 @@
       <c r="Z66" s="76"/>
     </row>
     <row r="67" spans="1:26" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A67" s="202" t="s">
+      <c r="A67" s="163" t="s">
         <v>26</v>
       </c>
-      <c r="B67" s="171">
+      <c r="B67" s="164">
         <v>255255255128</v>
       </c>
       <c r="C67" s="54" t="s">
         <v>212</v>
       </c>
-      <c r="D67" s="203">
+      <c r="D67" s="165">
         <v>2</v>
       </c>
-      <c r="E67" s="202">
+      <c r="E67" s="163">
         <v>126</v>
       </c>
       <c r="R67" s="73" t="s">
@@ -7465,13 +7472,13 @@
       <c r="Z67" s="148"/>
     </row>
     <row r="68" spans="1:26" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A68" s="169"/>
-      <c r="B68" s="172"/>
+      <c r="A68" s="150"/>
+      <c r="B68" s="152"/>
       <c r="C68" s="55">
         <v>1.1111111111111101E+31</v>
       </c>
-      <c r="D68" s="187"/>
-      <c r="E68" s="169"/>
+      <c r="D68" s="154"/>
+      <c r="E68" s="150"/>
       <c r="R68" s="73" t="s">
         <v>357</v>
       </c>
@@ -7484,19 +7491,19 @@
       <c r="Z68" s="72"/>
     </row>
     <row r="69" spans="1:26" x14ac:dyDescent="0.35">
-      <c r="A69" s="188" t="s">
+      <c r="A69" s="155" t="s">
         <v>27</v>
       </c>
-      <c r="B69" s="175">
+      <c r="B69" s="157">
         <v>255255255192</v>
       </c>
       <c r="C69" s="56" t="s">
         <v>213</v>
       </c>
-      <c r="D69" s="190">
+      <c r="D69" s="159">
         <v>4</v>
       </c>
-      <c r="E69" s="188">
+      <c r="E69" s="155">
         <v>62</v>
       </c>
       <c r="R69" s="73" t="s">
@@ -7511,13 +7518,13 @@
       <c r="Z69" s="74"/>
     </row>
     <row r="70" spans="1:26" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A70" s="189"/>
-      <c r="B70" s="176"/>
+      <c r="A70" s="156"/>
+      <c r="B70" s="158"/>
       <c r="C70" s="57">
         <v>1.1111111111111101E+31</v>
       </c>
-      <c r="D70" s="191"/>
-      <c r="E70" s="189"/>
+      <c r="D70" s="160"/>
+      <c r="E70" s="156"/>
       <c r="R70" s="73" t="s">
         <v>359</v>
       </c>
@@ -7530,19 +7537,19 @@
       <c r="Z70" s="76"/>
     </row>
     <row r="71" spans="1:26" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A71" s="168" t="s">
+      <c r="A71" s="149" t="s">
         <v>28</v>
       </c>
-      <c r="B71" s="185">
+      <c r="B71" s="151">
         <v>255255255224</v>
       </c>
       <c r="C71" s="58" t="s">
         <v>214</v>
       </c>
-      <c r="D71" s="186">
+      <c r="D71" s="153">
         <v>8</v>
       </c>
-      <c r="E71" s="168">
+      <c r="E71" s="149">
         <v>30</v>
       </c>
       <c r="R71" s="73" t="s">
@@ -7559,13 +7566,13 @@
       <c r="Z71" s="148"/>
     </row>
     <row r="72" spans="1:26" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A72" s="169"/>
-      <c r="B72" s="172"/>
+      <c r="A72" s="150"/>
+      <c r="B72" s="152"/>
       <c r="C72" s="55">
         <v>1.1111111111111101E+31</v>
       </c>
-      <c r="D72" s="187"/>
-      <c r="E72" s="169"/>
+      <c r="D72" s="154"/>
+      <c r="E72" s="150"/>
       <c r="R72" s="73" t="s">
         <v>361</v>
       </c>
@@ -7578,19 +7585,19 @@
       <c r="Z72" s="72"/>
     </row>
     <row r="73" spans="1:26" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A73" s="188" t="s">
+      <c r="A73" s="155" t="s">
         <v>29</v>
       </c>
-      <c r="B73" s="175">
+      <c r="B73" s="157">
         <v>255255255240</v>
       </c>
       <c r="C73" s="56" t="s">
         <v>215</v>
       </c>
-      <c r="D73" s="190">
+      <c r="D73" s="159">
         <v>16</v>
       </c>
-      <c r="E73" s="188">
+      <c r="E73" s="155">
         <v>14</v>
       </c>
       <c r="R73" s="75" t="s">
@@ -7605,13 +7612,13 @@
       <c r="Z73" s="74"/>
     </row>
     <row r="74" spans="1:26" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A74" s="189"/>
-      <c r="B74" s="176"/>
+      <c r="A74" s="156"/>
+      <c r="B74" s="158"/>
       <c r="C74" s="57">
         <v>1.1111111111111101E+31</v>
       </c>
-      <c r="D74" s="191"/>
-      <c r="E74" s="189"/>
+      <c r="D74" s="160"/>
+      <c r="E74" s="156"/>
       <c r="R74" s="146" t="s">
         <v>271</v>
       </c>
@@ -7622,19 +7629,19 @@
       <c r="Z74" s="76"/>
     </row>
     <row r="75" spans="1:26" x14ac:dyDescent="0.35">
-      <c r="A75" s="168" t="s">
+      <c r="A75" s="149" t="s">
         <v>30</v>
       </c>
-      <c r="B75" s="185">
+      <c r="B75" s="151">
         <v>255255255248</v>
       </c>
       <c r="C75" s="58" t="s">
         <v>216</v>
       </c>
-      <c r="D75" s="186">
+      <c r="D75" s="153">
         <v>32</v>
       </c>
-      <c r="E75" s="168">
+      <c r="E75" s="149">
         <v>6</v>
       </c>
       <c r="R75" s="71" t="s">
@@ -7645,13 +7652,13 @@
       </c>
     </row>
     <row r="76" spans="1:26" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A76" s="169"/>
-      <c r="B76" s="172"/>
+      <c r="A76" s="150"/>
+      <c r="B76" s="152"/>
       <c r="C76" s="55">
         <v>1.1111111111111101E+31</v>
       </c>
-      <c r="D76" s="187"/>
-      <c r="E76" s="169"/>
+      <c r="D76" s="154"/>
+      <c r="E76" s="150"/>
       <c r="R76" s="73" t="s">
         <v>364</v>
       </c>
@@ -7660,19 +7667,19 @@
       </c>
     </row>
     <row r="77" spans="1:26" x14ac:dyDescent="0.35">
-      <c r="A77" s="188" t="s">
+      <c r="A77" s="155" t="s">
         <v>31</v>
       </c>
-      <c r="B77" s="175">
+      <c r="B77" s="157">
         <v>255255255252</v>
       </c>
       <c r="C77" s="56" t="s">
         <v>217</v>
       </c>
-      <c r="D77" s="190">
+      <c r="D77" s="159">
         <v>64</v>
       </c>
-      <c r="E77" s="188">
+      <c r="E77" s="155">
         <v>2</v>
       </c>
       <c r="R77" s="73" t="s">
@@ -7683,13 +7690,13 @@
       </c>
     </row>
     <row r="78" spans="1:26" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A78" s="189"/>
-      <c r="B78" s="176"/>
+      <c r="A78" s="156"/>
+      <c r="B78" s="158"/>
       <c r="C78" s="57">
         <v>1.1111111111111101E+31</v>
       </c>
-      <c r="D78" s="191"/>
-      <c r="E78" s="189"/>
+      <c r="D78" s="160"/>
+      <c r="E78" s="156"/>
       <c r="R78" s="73" t="s">
         <v>366</v>
       </c>
@@ -7739,7 +7746,7 @@
       <c r="B83" s="46" t="s">
         <v>150</v>
       </c>
-      <c r="C83" s="200" t="s">
+      <c r="C83" s="161" t="s">
         <v>87</v>
       </c>
     </row>
@@ -7750,7 +7757,7 @@
       <c r="B84" s="47" t="s">
         <v>151</v>
       </c>
-      <c r="C84" s="201"/>
+      <c r="C84" s="162"/>
     </row>
     <row r="85" spans="1:19" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A85" s="48" t="s">
@@ -7870,7 +7877,7 @@
       <c r="B96" s="46" t="s">
         <v>150</v>
       </c>
-      <c r="C96" s="200" t="s">
+      <c r="C96" s="161" t="s">
         <v>87</v>
       </c>
     </row>
@@ -7881,7 +7888,7 @@
       <c r="B97" s="47" t="s">
         <v>180</v>
       </c>
-      <c r="C97" s="201"/>
+      <c r="C97" s="162"/>
     </row>
     <row r="98" spans="1:5" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A98" s="48" t="s">
@@ -8017,195 +8024,195 @@
     </row>
     <row r="111" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="112" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A112" s="200" t="s">
+      <c r="A112" s="161" t="s">
         <v>76</v>
       </c>
-      <c r="B112" s="200" t="s">
+      <c r="B112" s="161" t="s">
         <v>35</v>
       </c>
       <c r="C112" s="46" t="s">
         <v>209</v>
       </c>
-      <c r="D112" s="200" t="s">
+      <c r="D112" s="161" t="s">
         <v>211</v>
       </c>
-      <c r="E112" s="200" t="s">
+      <c r="E112" s="161" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="113" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A113" s="201"/>
-      <c r="B113" s="201"/>
+      <c r="A113" s="162"/>
+      <c r="B113" s="162"/>
       <c r="C113" s="52" t="s">
         <v>210</v>
       </c>
-      <c r="D113" s="201"/>
-      <c r="E113" s="201"/>
+      <c r="D113" s="162"/>
+      <c r="E113" s="162"/>
     </row>
     <row r="114" spans="1:5" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A114" s="202" t="s">
+      <c r="A114" s="163" t="s">
         <v>26</v>
       </c>
-      <c r="B114" s="171">
+      <c r="B114" s="164">
         <v>255255255128</v>
       </c>
       <c r="C114" s="54" t="s">
         <v>212</v>
       </c>
-      <c r="D114" s="203">
+      <c r="D114" s="165">
         <v>2</v>
       </c>
-      <c r="E114" s="202">
+      <c r="E114" s="163">
         <v>126</v>
       </c>
     </row>
     <row r="115" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A115" s="169"/>
-      <c r="B115" s="172"/>
+      <c r="A115" s="150"/>
+      <c r="B115" s="152"/>
       <c r="C115" s="55">
         <v>1.1111111111111101E+31</v>
       </c>
-      <c r="D115" s="187"/>
-      <c r="E115" s="169"/>
+      <c r="D115" s="154"/>
+      <c r="E115" s="150"/>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A116" s="188" t="s">
+      <c r="A116" s="155" t="s">
         <v>27</v>
       </c>
-      <c r="B116" s="175">
+      <c r="B116" s="157">
         <v>255255255192</v>
       </c>
       <c r="C116" s="56" t="s">
         <v>213</v>
       </c>
-      <c r="D116" s="190">
+      <c r="D116" s="159">
         <v>4</v>
       </c>
-      <c r="E116" s="188">
+      <c r="E116" s="155">
         <v>62</v>
       </c>
     </row>
     <row r="117" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A117" s="189"/>
-      <c r="B117" s="176"/>
+      <c r="A117" s="156"/>
+      <c r="B117" s="158"/>
       <c r="C117" s="57">
         <v>1.1111111111111101E+31</v>
       </c>
-      <c r="D117" s="191"/>
-      <c r="E117" s="189"/>
+      <c r="D117" s="160"/>
+      <c r="E117" s="156"/>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A118" s="168" t="s">
+      <c r="A118" s="149" t="s">
         <v>28</v>
       </c>
-      <c r="B118" s="185">
+      <c r="B118" s="151">
         <v>255255255224</v>
       </c>
       <c r="C118" s="58" t="s">
         <v>214</v>
       </c>
-      <c r="D118" s="186">
+      <c r="D118" s="153">
         <v>8</v>
       </c>
-      <c r="E118" s="168">
+      <c r="E118" s="149">
         <v>30</v>
       </c>
     </row>
     <row r="119" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A119" s="169"/>
-      <c r="B119" s="172"/>
+      <c r="A119" s="150"/>
+      <c r="B119" s="152"/>
       <c r="C119" s="55">
         <v>1.1111111111111101E+31</v>
       </c>
-      <c r="D119" s="187"/>
-      <c r="E119" s="169"/>
+      <c r="D119" s="154"/>
+      <c r="E119" s="150"/>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A120" s="188" t="s">
+      <c r="A120" s="155" t="s">
         <v>29</v>
       </c>
-      <c r="B120" s="175">
+      <c r="B120" s="157">
         <v>255255255240</v>
       </c>
       <c r="C120" s="56" t="s">
         <v>215</v>
       </c>
-      <c r="D120" s="190">
+      <c r="D120" s="159">
         <v>16</v>
       </c>
-      <c r="E120" s="188">
+      <c r="E120" s="155">
         <v>14</v>
       </c>
     </row>
     <row r="121" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A121" s="189"/>
-      <c r="B121" s="176"/>
+      <c r="A121" s="156"/>
+      <c r="B121" s="158"/>
       <c r="C121" s="57">
         <v>1.1111111111111101E+31</v>
       </c>
-      <c r="D121" s="191"/>
-      <c r="E121" s="189"/>
+      <c r="D121" s="160"/>
+      <c r="E121" s="156"/>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A122" s="168" t="s">
+      <c r="A122" s="149" t="s">
         <v>30</v>
       </c>
-      <c r="B122" s="185">
+      <c r="B122" s="151">
         <v>255255255248</v>
       </c>
       <c r="C122" s="58" t="s">
         <v>216</v>
       </c>
-      <c r="D122" s="186">
+      <c r="D122" s="153">
         <v>32</v>
       </c>
-      <c r="E122" s="168">
+      <c r="E122" s="149">
         <v>6</v>
       </c>
     </row>
     <row r="123" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A123" s="169"/>
-      <c r="B123" s="172"/>
+      <c r="A123" s="150"/>
+      <c r="B123" s="152"/>
       <c r="C123" s="55">
         <v>1.1111111111111101E+31</v>
       </c>
-      <c r="D123" s="187"/>
-      <c r="E123" s="169"/>
+      <c r="D123" s="154"/>
+      <c r="E123" s="150"/>
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A124" s="188" t="s">
+      <c r="A124" s="155" t="s">
         <v>31</v>
       </c>
-      <c r="B124" s="175">
+      <c r="B124" s="157">
         <v>255255255252</v>
       </c>
       <c r="C124" s="56" t="s">
         <v>217</v>
       </c>
-      <c r="D124" s="190">
+      <c r="D124" s="159">
         <v>64</v>
       </c>
-      <c r="E124" s="188">
+      <c r="E124" s="155">
         <v>2</v>
       </c>
     </row>
     <row r="125" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A125" s="189"/>
-      <c r="B125" s="176"/>
+      <c r="A125" s="156"/>
+      <c r="B125" s="158"/>
       <c r="C125" s="57">
         <v>1.1111111111111101E+31</v>
       </c>
-      <c r="D125" s="191"/>
-      <c r="E125" s="189"/>
+      <c r="D125" s="160"/>
+      <c r="E125" s="156"/>
     </row>
     <row r="127" spans="1:5" ht="20.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A127" s="192" t="s">
+      <c r="A127" s="180" t="s">
         <v>249</v>
       </c>
-      <c r="B127" s="193"/>
-      <c r="C127" s="193"/>
-      <c r="D127" s="193"/>
-      <c r="E127" s="193"/>
+      <c r="B127" s="181"/>
+      <c r="C127" s="181"/>
+      <c r="D127" s="181"/>
+      <c r="E127" s="181"/>
     </row>
     <row r="128" spans="1:5" ht="21.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A128" s="59" t="s">
@@ -8225,10 +8232,10 @@
       </c>
     </row>
     <row r="129" spans="1:5" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A129" s="177" t="s">
+      <c r="A129" s="178" t="s">
         <v>219</v>
       </c>
-      <c r="B129" s="177" t="s">
+      <c r="B129" s="178" t="s">
         <v>220</v>
       </c>
       <c r="C129" s="60" t="s">
@@ -8237,375 +8244,483 @@
       <c r="D129" s="179">
         <v>2</v>
       </c>
-      <c r="E129" s="177">
+      <c r="E129" s="178">
         <v>32766</v>
       </c>
     </row>
     <row r="130" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A130" s="178"/>
-      <c r="B130" s="178"/>
+      <c r="A130" s="167"/>
+      <c r="B130" s="167"/>
       <c r="C130" s="61">
         <v>1.1111111111111101E+31</v>
       </c>
-      <c r="D130" s="180"/>
-      <c r="E130" s="178"/>
+      <c r="D130" s="171"/>
+      <c r="E130" s="167"/>
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A131" s="181" t="s">
+      <c r="A131" s="172" t="s">
         <v>222</v>
       </c>
-      <c r="B131" s="181" t="s">
+      <c r="B131" s="172" t="s">
         <v>223</v>
       </c>
       <c r="C131" s="62" t="s">
         <v>224</v>
       </c>
-      <c r="D131" s="183">
+      <c r="D131" s="176">
         <v>4</v>
       </c>
-      <c r="E131" s="181">
+      <c r="E131" s="172">
         <v>16382</v>
       </c>
     </row>
     <row r="132" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A132" s="182"/>
-      <c r="B132" s="182"/>
+      <c r="A132" s="173"/>
+      <c r="B132" s="173"/>
       <c r="C132" s="63">
         <v>1.11111111111111E+29</v>
       </c>
-      <c r="D132" s="184"/>
-      <c r="E132" s="182"/>
+      <c r="D132" s="177"/>
+      <c r="E132" s="173"/>
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A133" s="194" t="s">
+      <c r="A133" s="166" t="s">
         <v>225</v>
       </c>
-      <c r="B133" s="194" t="s">
+      <c r="B133" s="166" t="s">
         <v>226</v>
       </c>
       <c r="C133" s="64" t="s">
         <v>227</v>
       </c>
-      <c r="D133" s="195">
+      <c r="D133" s="170">
         <v>8</v>
       </c>
-      <c r="E133" s="194">
+      <c r="E133" s="166">
         <v>8190</v>
       </c>
     </row>
     <row r="134" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A134" s="178"/>
-      <c r="B134" s="178"/>
+      <c r="A134" s="167"/>
+      <c r="B134" s="167"/>
       <c r="C134" s="61">
         <v>1.11111111111111E+29</v>
       </c>
-      <c r="D134" s="180"/>
-      <c r="E134" s="178"/>
+      <c r="D134" s="171"/>
+      <c r="E134" s="167"/>
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A135" s="181" t="s">
+      <c r="A135" s="172" t="s">
         <v>228</v>
       </c>
-      <c r="B135" s="181" t="s">
+      <c r="B135" s="172" t="s">
         <v>229</v>
       </c>
       <c r="C135" s="62" t="s">
         <v>230</v>
       </c>
-      <c r="D135" s="183">
+      <c r="D135" s="176">
         <v>16</v>
       </c>
-      <c r="E135" s="181">
+      <c r="E135" s="172">
         <v>4094</v>
       </c>
     </row>
     <row r="136" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A136" s="182"/>
-      <c r="B136" s="182"/>
+      <c r="A136" s="173"/>
+      <c r="B136" s="173"/>
       <c r="C136" s="63">
         <v>1.11111111111111E+29</v>
       </c>
-      <c r="D136" s="184"/>
-      <c r="E136" s="182"/>
+      <c r="D136" s="177"/>
+      <c r="E136" s="173"/>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A137" s="194" t="s">
+      <c r="A137" s="166" t="s">
         <v>231</v>
       </c>
-      <c r="B137" s="194" t="s">
+      <c r="B137" s="166" t="s">
         <v>232</v>
       </c>
       <c r="C137" s="64" t="s">
         <v>233</v>
       </c>
-      <c r="D137" s="195">
+      <c r="D137" s="170">
         <v>32</v>
       </c>
-      <c r="E137" s="194">
+      <c r="E137" s="166">
         <v>2046</v>
       </c>
     </row>
     <row r="138" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A138" s="178"/>
-      <c r="B138" s="178"/>
+      <c r="A138" s="167"/>
+      <c r="B138" s="167"/>
       <c r="C138" s="61">
         <v>1.11111111111111E+29</v>
       </c>
-      <c r="D138" s="180"/>
-      <c r="E138" s="178"/>
+      <c r="D138" s="171"/>
+      <c r="E138" s="167"/>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A139" s="181" t="s">
+      <c r="A139" s="172" t="s">
         <v>234</v>
       </c>
-      <c r="B139" s="181" t="s">
+      <c r="B139" s="172" t="s">
         <v>235</v>
       </c>
       <c r="C139" s="62" t="s">
         <v>236</v>
       </c>
-      <c r="D139" s="183">
+      <c r="D139" s="176">
         <v>64</v>
       </c>
-      <c r="E139" s="181">
+      <c r="E139" s="172">
         <v>1022</v>
       </c>
     </row>
     <row r="140" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A140" s="182"/>
-      <c r="B140" s="182"/>
+      <c r="A140" s="173"/>
+      <c r="B140" s="173"/>
       <c r="C140" s="63">
         <v>1.11111111111111E+29</v>
       </c>
-      <c r="D140" s="184"/>
-      <c r="E140" s="182"/>
+      <c r="D140" s="177"/>
+      <c r="E140" s="173"/>
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A141" s="194" t="s">
+      <c r="A141" s="166" t="s">
         <v>237</v>
       </c>
-      <c r="B141" s="194" t="s">
+      <c r="B141" s="166" t="s">
         <v>238</v>
       </c>
       <c r="C141" s="64" t="s">
         <v>239</v>
       </c>
-      <c r="D141" s="195">
+      <c r="D141" s="170">
         <v>128</v>
       </c>
-      <c r="E141" s="194">
+      <c r="E141" s="166">
         <v>510</v>
       </c>
     </row>
     <row r="142" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A142" s="178"/>
-      <c r="B142" s="178"/>
+      <c r="A142" s="167"/>
+      <c r="B142" s="167"/>
       <c r="C142" s="61">
         <v>1.11111111111111E+29</v>
       </c>
-      <c r="D142" s="180"/>
-      <c r="E142" s="178"/>
+      <c r="D142" s="171"/>
+      <c r="E142" s="167"/>
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A143" s="181" t="s">
+      <c r="A143" s="172" t="s">
         <v>25</v>
       </c>
-      <c r="B143" s="181" t="s">
+      <c r="B143" s="172" t="s">
         <v>240</v>
       </c>
       <c r="C143" s="62" t="s">
         <v>241</v>
       </c>
-      <c r="D143" s="183">
+      <c r="D143" s="176">
         <v>256</v>
       </c>
-      <c r="E143" s="181">
+      <c r="E143" s="172">
         <v>254</v>
       </c>
     </row>
     <row r="144" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A144" s="182"/>
-      <c r="B144" s="182"/>
+      <c r="A144" s="173"/>
+      <c r="B144" s="173"/>
       <c r="C144" s="63">
         <v>1.11111111111111E+29</v>
       </c>
-      <c r="D144" s="184"/>
-      <c r="E144" s="182"/>
+      <c r="D144" s="177"/>
+      <c r="E144" s="173"/>
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A145" s="194" t="s">
+      <c r="A145" s="166" t="s">
         <v>26</v>
       </c>
-      <c r="B145" s="196">
+      <c r="B145" s="168">
         <v>255255255128</v>
       </c>
       <c r="C145" s="64" t="s">
         <v>242</v>
       </c>
-      <c r="D145" s="195">
+      <c r="D145" s="170">
         <v>512</v>
       </c>
-      <c r="E145" s="194">
+      <c r="E145" s="166">
         <v>126</v>
       </c>
     </row>
     <row r="146" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A146" s="178"/>
-      <c r="B146" s="197"/>
+      <c r="A146" s="167"/>
+      <c r="B146" s="169"/>
       <c r="C146" s="61">
         <v>1.11111111111111E+29</v>
       </c>
-      <c r="D146" s="180"/>
-      <c r="E146" s="178"/>
+      <c r="D146" s="171"/>
+      <c r="E146" s="167"/>
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A147" s="181" t="s">
+      <c r="A147" s="172" t="s">
         <v>27</v>
       </c>
-      <c r="B147" s="198">
+      <c r="B147" s="174">
         <v>255255255192</v>
       </c>
       <c r="C147" s="62" t="s">
         <v>243</v>
       </c>
-      <c r="D147" s="183">
+      <c r="D147" s="176">
         <v>1024</v>
       </c>
-      <c r="E147" s="181">
+      <c r="E147" s="172">
         <v>62</v>
       </c>
     </row>
     <row r="148" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A148" s="182"/>
-      <c r="B148" s="199"/>
+      <c r="A148" s="173"/>
+      <c r="B148" s="175"/>
       <c r="C148" s="63">
         <v>1.11111111111111E+29</v>
       </c>
-      <c r="D148" s="184"/>
-      <c r="E148" s="182"/>
+      <c r="D148" s="177"/>
+      <c r="E148" s="173"/>
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A149" s="194" t="s">
+      <c r="A149" s="166" t="s">
         <v>28</v>
       </c>
-      <c r="B149" s="196">
+      <c r="B149" s="168">
         <v>255255255224</v>
       </c>
       <c r="C149" s="64" t="s">
         <v>244</v>
       </c>
-      <c r="D149" s="195">
+      <c r="D149" s="170">
         <v>2048</v>
       </c>
-      <c r="E149" s="194">
+      <c r="E149" s="166">
         <v>30</v>
       </c>
     </row>
     <row r="150" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A150" s="178"/>
-      <c r="B150" s="197"/>
+      <c r="A150" s="167"/>
+      <c r="B150" s="169"/>
       <c r="C150" s="61">
         <v>1.11111111111111E+29</v>
       </c>
-      <c r="D150" s="180"/>
-      <c r="E150" s="178"/>
+      <c r="D150" s="171"/>
+      <c r="E150" s="167"/>
     </row>
     <row r="151" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A151" s="181" t="s">
+      <c r="A151" s="172" t="s">
         <v>29</v>
       </c>
-      <c r="B151" s="181" t="s">
+      <c r="B151" s="172" t="s">
         <v>245</v>
       </c>
       <c r="C151" s="62" t="s">
         <v>246</v>
       </c>
-      <c r="D151" s="183">
+      <c r="D151" s="176">
         <v>4096</v>
       </c>
-      <c r="E151" s="181">
+      <c r="E151" s="172">
         <v>14</v>
       </c>
     </row>
     <row r="152" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A152" s="182"/>
-      <c r="B152" s="182"/>
+      <c r="A152" s="173"/>
+      <c r="B152" s="173"/>
       <c r="C152" s="63">
         <v>1.11111111111111E+29</v>
       </c>
-      <c r="D152" s="184"/>
-      <c r="E152" s="182"/>
+      <c r="D152" s="177"/>
+      <c r="E152" s="173"/>
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A153" s="194" t="s">
+      <c r="A153" s="166" t="s">
         <v>30</v>
       </c>
-      <c r="B153" s="196">
+      <c r="B153" s="168">
         <v>255255255248</v>
       </c>
       <c r="C153" s="64" t="s">
         <v>247</v>
       </c>
-      <c r="D153" s="195">
+      <c r="D153" s="170">
         <v>8192</v>
       </c>
-      <c r="E153" s="194">
+      <c r="E153" s="166">
         <v>6</v>
       </c>
     </row>
     <row r="154" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A154" s="178"/>
-      <c r="B154" s="197"/>
+      <c r="A154" s="167"/>
+      <c r="B154" s="169"/>
       <c r="C154" s="61">
         <v>1.11111111111111E+29</v>
       </c>
-      <c r="D154" s="180"/>
-      <c r="E154" s="178"/>
+      <c r="D154" s="171"/>
+      <c r="E154" s="167"/>
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A155" s="181" t="s">
+      <c r="A155" s="172" t="s">
         <v>31</v>
       </c>
-      <c r="B155" s="198">
+      <c r="B155" s="174">
         <v>255255255252</v>
       </c>
       <c r="C155" s="62" t="s">
         <v>248</v>
       </c>
-      <c r="D155" s="183">
+      <c r="D155" s="176">
         <v>16384</v>
       </c>
-      <c r="E155" s="181">
+      <c r="E155" s="172">
         <v>2</v>
       </c>
     </row>
     <row r="156" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A156" s="182"/>
-      <c r="B156" s="199"/>
+      <c r="A156" s="173"/>
+      <c r="B156" s="175"/>
       <c r="C156" s="63">
         <v>1.11111111111111E+27</v>
       </c>
-      <c r="D156" s="184"/>
-      <c r="E156" s="182"/>
+      <c r="D156" s="177"/>
+      <c r="E156" s="173"/>
     </row>
   </sheetData>
   <mergeCells count="164">
-    <mergeCell ref="Y67:Z67"/>
-    <mergeCell ref="Y71:Z71"/>
-    <mergeCell ref="A71:A72"/>
-    <mergeCell ref="B71:B72"/>
-    <mergeCell ref="D71:D72"/>
-    <mergeCell ref="A118:A119"/>
-    <mergeCell ref="B118:B119"/>
-    <mergeCell ref="D118:D119"/>
-    <mergeCell ref="E118:E119"/>
-    <mergeCell ref="E71:E72"/>
-    <mergeCell ref="A73:A74"/>
-    <mergeCell ref="B73:B74"/>
-    <mergeCell ref="D73:D74"/>
-    <mergeCell ref="E73:E74"/>
-    <mergeCell ref="D112:D113"/>
-    <mergeCell ref="E112:E113"/>
+    <mergeCell ref="R38:S38"/>
+    <mergeCell ref="R47:S47"/>
+    <mergeCell ref="R56:S56"/>
+    <mergeCell ref="R65:S65"/>
+    <mergeCell ref="R74:S74"/>
+    <mergeCell ref="AA24:AB24"/>
+    <mergeCell ref="AA29:AB29"/>
+    <mergeCell ref="Y26:Z26"/>
+    <mergeCell ref="R1:Z1"/>
+    <mergeCell ref="U11:V11"/>
+    <mergeCell ref="R11:S11"/>
+    <mergeCell ref="Y19:Z19"/>
+    <mergeCell ref="U41:V41"/>
+    <mergeCell ref="U51:V51"/>
+    <mergeCell ref="U55:V55"/>
+    <mergeCell ref="U59:V59"/>
+    <mergeCell ref="U63:V63"/>
+    <mergeCell ref="U67:V67"/>
+    <mergeCell ref="U71:V71"/>
+    <mergeCell ref="AA34:AB34"/>
+    <mergeCell ref="Y51:Z51"/>
+    <mergeCell ref="Y55:Z55"/>
+    <mergeCell ref="Y59:Z59"/>
+    <mergeCell ref="Y63:Z63"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="F1:N1"/>
+    <mergeCell ref="Y10:AA10"/>
+    <mergeCell ref="R20:S20"/>
+    <mergeCell ref="R29:S29"/>
+    <mergeCell ref="U21:V21"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="D15:D16"/>
+    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="D19:D20"/>
+    <mergeCell ref="D21:D22"/>
+    <mergeCell ref="D23:D24"/>
+    <mergeCell ref="U31:V31"/>
+    <mergeCell ref="A59:A60"/>
+    <mergeCell ref="B59:B60"/>
+    <mergeCell ref="D59:D60"/>
+    <mergeCell ref="A55:A56"/>
+    <mergeCell ref="B55:B56"/>
+    <mergeCell ref="D55:D56"/>
+    <mergeCell ref="A57:A58"/>
+    <mergeCell ref="B57:B58"/>
+    <mergeCell ref="D57:D58"/>
+    <mergeCell ref="A129:A130"/>
+    <mergeCell ref="B129:B130"/>
+    <mergeCell ref="D129:D130"/>
+    <mergeCell ref="E129:E130"/>
+    <mergeCell ref="A131:A132"/>
+    <mergeCell ref="B131:B132"/>
+    <mergeCell ref="D131:D132"/>
+    <mergeCell ref="E131:E132"/>
+    <mergeCell ref="A122:A123"/>
+    <mergeCell ref="B122:B123"/>
+    <mergeCell ref="D122:D123"/>
+    <mergeCell ref="E122:E123"/>
+    <mergeCell ref="A124:A125"/>
+    <mergeCell ref="B124:B125"/>
+    <mergeCell ref="D124:D125"/>
+    <mergeCell ref="E124:E125"/>
+    <mergeCell ref="A127:E127"/>
+    <mergeCell ref="A137:A138"/>
+    <mergeCell ref="B137:B138"/>
+    <mergeCell ref="D137:D138"/>
+    <mergeCell ref="E137:E138"/>
+    <mergeCell ref="A139:A140"/>
+    <mergeCell ref="B139:B140"/>
+    <mergeCell ref="D139:D140"/>
+    <mergeCell ref="E139:E140"/>
+    <mergeCell ref="A133:A134"/>
+    <mergeCell ref="B133:B134"/>
+    <mergeCell ref="D133:D134"/>
+    <mergeCell ref="E133:E134"/>
+    <mergeCell ref="A135:A136"/>
+    <mergeCell ref="B135:B136"/>
+    <mergeCell ref="D135:D136"/>
+    <mergeCell ref="E135:E136"/>
+    <mergeCell ref="A145:A146"/>
+    <mergeCell ref="B145:B146"/>
+    <mergeCell ref="D145:D146"/>
+    <mergeCell ref="E145:E146"/>
+    <mergeCell ref="A147:A148"/>
+    <mergeCell ref="B147:B148"/>
+    <mergeCell ref="D147:D148"/>
+    <mergeCell ref="E147:E148"/>
+    <mergeCell ref="A141:A142"/>
+    <mergeCell ref="B141:B142"/>
+    <mergeCell ref="D141:D142"/>
+    <mergeCell ref="E141:E142"/>
+    <mergeCell ref="A143:A144"/>
+    <mergeCell ref="B143:B144"/>
+    <mergeCell ref="D143:D144"/>
+    <mergeCell ref="E143:E144"/>
+    <mergeCell ref="A153:A154"/>
+    <mergeCell ref="B153:B154"/>
+    <mergeCell ref="D153:D154"/>
+    <mergeCell ref="E153:E154"/>
+    <mergeCell ref="A155:A156"/>
+    <mergeCell ref="B155:B156"/>
+    <mergeCell ref="D155:D156"/>
+    <mergeCell ref="E155:E156"/>
+    <mergeCell ref="A149:A150"/>
+    <mergeCell ref="B149:B150"/>
+    <mergeCell ref="D149:D150"/>
+    <mergeCell ref="E149:E150"/>
+    <mergeCell ref="A151:A152"/>
+    <mergeCell ref="B151:B152"/>
+    <mergeCell ref="D151:D152"/>
+    <mergeCell ref="E151:E152"/>
+    <mergeCell ref="A65:A66"/>
+    <mergeCell ref="B65:B66"/>
+    <mergeCell ref="D65:D66"/>
+    <mergeCell ref="E65:E66"/>
+    <mergeCell ref="A67:A68"/>
+    <mergeCell ref="B67:B68"/>
+    <mergeCell ref="D67:D68"/>
+    <mergeCell ref="E67:E68"/>
+    <mergeCell ref="A69:A70"/>
+    <mergeCell ref="B69:B70"/>
+    <mergeCell ref="D69:D70"/>
+    <mergeCell ref="E69:E70"/>
     <mergeCell ref="A120:A121"/>
     <mergeCell ref="B120:B121"/>
     <mergeCell ref="D120:D121"/>
@@ -8630,130 +8745,22 @@
     <mergeCell ref="C96:C97"/>
     <mergeCell ref="A112:A113"/>
     <mergeCell ref="B112:B113"/>
-    <mergeCell ref="A65:A66"/>
-    <mergeCell ref="B65:B66"/>
-    <mergeCell ref="D65:D66"/>
-    <mergeCell ref="E65:E66"/>
-    <mergeCell ref="A67:A68"/>
-    <mergeCell ref="B67:B68"/>
-    <mergeCell ref="D67:D68"/>
-    <mergeCell ref="E67:E68"/>
-    <mergeCell ref="A69:A70"/>
-    <mergeCell ref="B69:B70"/>
-    <mergeCell ref="D69:D70"/>
-    <mergeCell ref="E69:E70"/>
-    <mergeCell ref="A153:A154"/>
-    <mergeCell ref="B153:B154"/>
-    <mergeCell ref="D153:D154"/>
-    <mergeCell ref="E153:E154"/>
-    <mergeCell ref="A155:A156"/>
-    <mergeCell ref="B155:B156"/>
-    <mergeCell ref="D155:D156"/>
-    <mergeCell ref="E155:E156"/>
-    <mergeCell ref="A149:A150"/>
-    <mergeCell ref="B149:B150"/>
-    <mergeCell ref="D149:D150"/>
-    <mergeCell ref="E149:E150"/>
-    <mergeCell ref="A151:A152"/>
-    <mergeCell ref="B151:B152"/>
-    <mergeCell ref="D151:D152"/>
-    <mergeCell ref="E151:E152"/>
-    <mergeCell ref="A145:A146"/>
-    <mergeCell ref="B145:B146"/>
-    <mergeCell ref="D145:D146"/>
-    <mergeCell ref="E145:E146"/>
-    <mergeCell ref="A147:A148"/>
-    <mergeCell ref="B147:B148"/>
-    <mergeCell ref="D147:D148"/>
-    <mergeCell ref="E147:E148"/>
-    <mergeCell ref="A141:A142"/>
-    <mergeCell ref="B141:B142"/>
-    <mergeCell ref="D141:D142"/>
-    <mergeCell ref="E141:E142"/>
-    <mergeCell ref="A143:A144"/>
-    <mergeCell ref="B143:B144"/>
-    <mergeCell ref="D143:D144"/>
-    <mergeCell ref="E143:E144"/>
-    <mergeCell ref="A137:A138"/>
-    <mergeCell ref="B137:B138"/>
-    <mergeCell ref="D137:D138"/>
-    <mergeCell ref="E137:E138"/>
-    <mergeCell ref="A139:A140"/>
-    <mergeCell ref="B139:B140"/>
-    <mergeCell ref="D139:D140"/>
-    <mergeCell ref="E139:E140"/>
-    <mergeCell ref="A133:A134"/>
-    <mergeCell ref="B133:B134"/>
-    <mergeCell ref="D133:D134"/>
-    <mergeCell ref="E133:E134"/>
-    <mergeCell ref="A135:A136"/>
-    <mergeCell ref="B135:B136"/>
-    <mergeCell ref="D135:D136"/>
-    <mergeCell ref="E135:E136"/>
-    <mergeCell ref="A129:A130"/>
-    <mergeCell ref="B129:B130"/>
-    <mergeCell ref="D129:D130"/>
-    <mergeCell ref="E129:E130"/>
-    <mergeCell ref="A131:A132"/>
-    <mergeCell ref="B131:B132"/>
-    <mergeCell ref="D131:D132"/>
-    <mergeCell ref="E131:E132"/>
-    <mergeCell ref="A122:A123"/>
-    <mergeCell ref="B122:B123"/>
-    <mergeCell ref="D122:D123"/>
-    <mergeCell ref="E122:E123"/>
-    <mergeCell ref="A124:A125"/>
-    <mergeCell ref="B124:B125"/>
-    <mergeCell ref="D124:D125"/>
-    <mergeCell ref="E124:E125"/>
-    <mergeCell ref="A127:E127"/>
-    <mergeCell ref="A59:A60"/>
-    <mergeCell ref="B59:B60"/>
-    <mergeCell ref="D59:D60"/>
-    <mergeCell ref="A55:A56"/>
-    <mergeCell ref="B55:B56"/>
-    <mergeCell ref="D55:D56"/>
-    <mergeCell ref="A57:A58"/>
-    <mergeCell ref="B57:B58"/>
-    <mergeCell ref="D57:D58"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="F1:N1"/>
-    <mergeCell ref="Y10:AA10"/>
-    <mergeCell ref="R20:S20"/>
-    <mergeCell ref="R29:S29"/>
-    <mergeCell ref="U21:V21"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="D15:D16"/>
-    <mergeCell ref="D17:D18"/>
-    <mergeCell ref="D19:D20"/>
-    <mergeCell ref="D21:D22"/>
-    <mergeCell ref="D23:D24"/>
-    <mergeCell ref="U31:V31"/>
-    <mergeCell ref="R38:S38"/>
-    <mergeCell ref="R47:S47"/>
-    <mergeCell ref="R56:S56"/>
-    <mergeCell ref="R65:S65"/>
-    <mergeCell ref="R74:S74"/>
-    <mergeCell ref="AA24:AB24"/>
-    <mergeCell ref="AA29:AB29"/>
-    <mergeCell ref="Y26:Z26"/>
-    <mergeCell ref="R1:Z1"/>
-    <mergeCell ref="U11:V11"/>
-    <mergeCell ref="R11:S11"/>
-    <mergeCell ref="Y19:Z19"/>
-    <mergeCell ref="U41:V41"/>
-    <mergeCell ref="U51:V51"/>
-    <mergeCell ref="U55:V55"/>
-    <mergeCell ref="U59:V59"/>
-    <mergeCell ref="U63:V63"/>
-    <mergeCell ref="U67:V67"/>
-    <mergeCell ref="U71:V71"/>
-    <mergeCell ref="AA34:AB34"/>
-    <mergeCell ref="Y51:Z51"/>
-    <mergeCell ref="Y55:Z55"/>
-    <mergeCell ref="Y59:Z59"/>
-    <mergeCell ref="Y63:Z63"/>
+    <mergeCell ref="Y67:Z67"/>
+    <mergeCell ref="Y71:Z71"/>
+    <mergeCell ref="A71:A72"/>
+    <mergeCell ref="B71:B72"/>
+    <mergeCell ref="D71:D72"/>
+    <mergeCell ref="A118:A119"/>
+    <mergeCell ref="B118:B119"/>
+    <mergeCell ref="D118:D119"/>
+    <mergeCell ref="E118:E119"/>
+    <mergeCell ref="E71:E72"/>
+    <mergeCell ref="A73:A74"/>
+    <mergeCell ref="B73:B74"/>
+    <mergeCell ref="D73:D74"/>
+    <mergeCell ref="E73:E74"/>
+    <mergeCell ref="D112:D113"/>
+    <mergeCell ref="E112:E113"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <drawing r:id="rId1"/>
@@ -8764,8 +8771,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82F3A8FF-CAC2-47FA-A920-5D12ECFC0104}">
   <dimension ref="A1:J86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="90" workbookViewId="0">
+      <selection activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -8782,67 +8789,67 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="204" t="s">
+      <c r="A1" s="210" t="s">
         <v>339</v>
       </c>
-      <c r="B1" s="205"/>
-      <c r="C1" s="205"/>
-      <c r="D1" s="205"/>
-      <c r="E1" s="205"/>
-      <c r="F1" s="205"/>
-      <c r="G1" s="205"/>
-      <c r="H1" s="205"/>
-      <c r="I1" s="205"/>
-      <c r="J1" s="206"/>
+      <c r="B1" s="211"/>
+      <c r="C1" s="211"/>
+      <c r="D1" s="211"/>
+      <c r="E1" s="211"/>
+      <c r="F1" s="211"/>
+      <c r="G1" s="211"/>
+      <c r="H1" s="211"/>
+      <c r="I1" s="211"/>
+      <c r="J1" s="212"/>
     </row>
     <row r="2" spans="1:10" ht="67.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="207" t="s">
+      <c r="A2" s="213" t="s">
         <v>130</v>
       </c>
-      <c r="B2" s="207" t="s">
+      <c r="B2" s="213" t="s">
         <v>131</v>
       </c>
-      <c r="C2" s="207" t="s">
+      <c r="C2" s="213" t="s">
         <v>147</v>
       </c>
-      <c r="D2" s="207" t="s">
+      <c r="D2" s="213" t="s">
         <v>132</v>
       </c>
-      <c r="E2" s="210" t="s">
+      <c r="E2" s="216" t="s">
         <v>16</v>
       </c>
-      <c r="F2" s="212" t="s">
+      <c r="F2" s="218" t="s">
         <v>133</v>
       </c>
-      <c r="G2" s="213"/>
-      <c r="H2" s="210" t="s">
+      <c r="G2" s="219"/>
+      <c r="H2" s="216" t="s">
         <v>134</v>
       </c>
-      <c r="I2" s="207" t="s">
+      <c r="I2" s="213" t="s">
         <v>135</v>
       </c>
-      <c r="J2" s="210" t="s">
+      <c r="J2" s="216" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="208"/>
-      <c r="B3" s="209"/>
-      <c r="C3" s="209"/>
-      <c r="D3" s="209"/>
-      <c r="E3" s="211"/>
+      <c r="A3" s="214"/>
+      <c r="B3" s="215"/>
+      <c r="C3" s="215"/>
+      <c r="D3" s="215"/>
+      <c r="E3" s="217"/>
       <c r="F3" s="93" t="s">
         <v>137</v>
       </c>
       <c r="G3" s="93" t="s">
         <v>138</v>
       </c>
-      <c r="H3" s="211"/>
-      <c r="I3" s="209"/>
-      <c r="J3" s="211"/>
+      <c r="H3" s="217"/>
+      <c r="I3" s="215"/>
+      <c r="J3" s="217"/>
     </row>
     <row r="4" spans="1:10" ht="15.65" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="217" t="s">
+      <c r="A4" s="207" t="s">
         <v>139</v>
       </c>
       <c r="B4" s="94" t="s">
@@ -8874,7 +8881,7 @@
       </c>
     </row>
     <row r="5" spans="1:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="218"/>
+      <c r="A5" s="208"/>
       <c r="B5" s="94" t="s">
         <v>308</v>
       </c>
@@ -8904,7 +8911,7 @@
       </c>
     </row>
     <row r="6" spans="1:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="218"/>
+      <c r="A6" s="208"/>
       <c r="B6" s="94" t="s">
         <v>309</v>
       </c>
@@ -8934,7 +8941,7 @@
       </c>
     </row>
     <row r="7" spans="1:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="218"/>
+      <c r="A7" s="208"/>
       <c r="B7" s="94" t="s">
         <v>310</v>
       </c>
@@ -8952,7 +8959,7 @@
       </c>
     </row>
     <row r="8" spans="1:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="218"/>
+      <c r="A8" s="208"/>
       <c r="B8" s="94" t="s">
         <v>311</v>
       </c>
@@ -8970,7 +8977,7 @@
       </c>
     </row>
     <row r="9" spans="1:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="218"/>
+      <c r="A9" s="208"/>
       <c r="B9" s="94" t="s">
         <v>312</v>
       </c>
@@ -8988,7 +8995,7 @@
       </c>
     </row>
     <row r="10" spans="1:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A10" s="218"/>
+      <c r="A10" s="208"/>
       <c r="B10" s="94" t="s">
         <v>313</v>
       </c>
@@ -9006,7 +9013,7 @@
       </c>
     </row>
     <row r="11" spans="1:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A11" s="218"/>
+      <c r="A11" s="208"/>
       <c r="B11" s="94" t="s">
         <v>315</v>
       </c>
@@ -9024,7 +9031,7 @@
       </c>
     </row>
     <row r="12" spans="1:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A12" s="218"/>
+      <c r="A12" s="208"/>
       <c r="B12" s="94" t="s">
         <v>314</v>
       </c>
@@ -9042,7 +9049,7 @@
       </c>
     </row>
     <row r="13" spans="1:10" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A13" s="219"/>
+      <c r="A13" s="209"/>
       <c r="B13" s="94" t="s">
         <v>316</v>
       </c>
@@ -9060,16 +9067,16 @@
       </c>
     </row>
     <row r="14" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A14" s="214"/>
-      <c r="B14" s="215"/>
-      <c r="C14" s="215"/>
-      <c r="D14" s="215"/>
-      <c r="E14" s="215"/>
-      <c r="F14" s="215"/>
-      <c r="G14" s="215"/>
-      <c r="H14" s="215"/>
-      <c r="I14" s="215"/>
-      <c r="J14" s="216"/>
+      <c r="A14" s="204"/>
+      <c r="B14" s="205"/>
+      <c r="C14" s="205"/>
+      <c r="D14" s="205"/>
+      <c r="E14" s="205"/>
+      <c r="F14" s="205"/>
+      <c r="G14" s="205"/>
+      <c r="H14" s="205"/>
+      <c r="I14" s="205"/>
+      <c r="J14" s="206"/>
     </row>
     <row r="15" spans="1:10" s="99" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A15" s="96" t="s">
@@ -9136,16 +9143,16 @@
       </c>
     </row>
     <row r="17" spans="1:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="214"/>
-      <c r="B17" s="215"/>
-      <c r="C17" s="215"/>
-      <c r="D17" s="215"/>
-      <c r="E17" s="215"/>
-      <c r="F17" s="215"/>
-      <c r="G17" s="215"/>
-      <c r="H17" s="215"/>
-      <c r="I17" s="215"/>
-      <c r="J17" s="216"/>
+      <c r="A17" s="204"/>
+      <c r="B17" s="205"/>
+      <c r="C17" s="205"/>
+      <c r="D17" s="205"/>
+      <c r="E17" s="205"/>
+      <c r="F17" s="205"/>
+      <c r="G17" s="205"/>
+      <c r="H17" s="205"/>
+      <c r="I17" s="205"/>
+      <c r="J17" s="206"/>
     </row>
     <row r="18" spans="1:10" s="99" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A18" s="101" t="s">
@@ -9212,16 +9219,16 @@
       </c>
     </row>
     <row r="20" spans="1:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A20" s="214"/>
-      <c r="B20" s="215"/>
-      <c r="C20" s="215"/>
-      <c r="D20" s="215"/>
-      <c r="E20" s="215"/>
-      <c r="F20" s="215"/>
-      <c r="G20" s="215"/>
-      <c r="H20" s="215"/>
-      <c r="I20" s="215"/>
-      <c r="J20" s="216"/>
+      <c r="A20" s="204"/>
+      <c r="B20" s="205"/>
+      <c r="C20" s="205"/>
+      <c r="D20" s="205"/>
+      <c r="E20" s="205"/>
+      <c r="F20" s="205"/>
+      <c r="G20" s="205"/>
+      <c r="H20" s="205"/>
+      <c r="I20" s="205"/>
+      <c r="J20" s="206"/>
     </row>
     <row r="21" spans="1:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A21" s="105" t="s">
@@ -9260,16 +9267,16 @@
       </c>
     </row>
     <row r="23" spans="1:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A23" s="214"/>
-      <c r="B23" s="215"/>
-      <c r="C23" s="215"/>
-      <c r="D23" s="215"/>
-      <c r="E23" s="215"/>
-      <c r="F23" s="215"/>
-      <c r="G23" s="215"/>
-      <c r="H23" s="215"/>
-      <c r="I23" s="215"/>
-      <c r="J23" s="216"/>
+      <c r="A23" s="204"/>
+      <c r="B23" s="205"/>
+      <c r="C23" s="205"/>
+      <c r="D23" s="205"/>
+      <c r="E23" s="205"/>
+      <c r="F23" s="205"/>
+      <c r="G23" s="205"/>
+      <c r="H23" s="205"/>
+      <c r="I23" s="205"/>
+      <c r="J23" s="206"/>
     </row>
     <row r="24" spans="1:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A24" s="109" t="s">
@@ -9308,16 +9315,16 @@
       </c>
     </row>
     <row r="26" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A26" s="214"/>
-      <c r="B26" s="215"/>
-      <c r="C26" s="215"/>
-      <c r="D26" s="215"/>
-      <c r="E26" s="215"/>
-      <c r="F26" s="215"/>
-      <c r="G26" s="215"/>
-      <c r="H26" s="215"/>
-      <c r="I26" s="215"/>
-      <c r="J26" s="216"/>
+      <c r="A26" s="204"/>
+      <c r="B26" s="205"/>
+      <c r="C26" s="205"/>
+      <c r="D26" s="205"/>
+      <c r="E26" s="205"/>
+      <c r="F26" s="205"/>
+      <c r="G26" s="205"/>
+      <c r="H26" s="205"/>
+      <c r="I26" s="205"/>
+      <c r="J26" s="206"/>
     </row>
     <row r="27" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A27" s="113" t="s">
@@ -9356,16 +9363,16 @@
       </c>
     </row>
     <row r="29" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A29" s="214"/>
-      <c r="B29" s="215"/>
-      <c r="C29" s="215"/>
-      <c r="D29" s="215"/>
-      <c r="E29" s="215"/>
-      <c r="F29" s="215"/>
-      <c r="G29" s="215"/>
-      <c r="H29" s="215"/>
-      <c r="I29" s="215"/>
-      <c r="J29" s="216"/>
+      <c r="A29" s="204"/>
+      <c r="B29" s="205"/>
+      <c r="C29" s="205"/>
+      <c r="D29" s="205"/>
+      <c r="E29" s="205"/>
+      <c r="F29" s="205"/>
+      <c r="G29" s="205"/>
+      <c r="H29" s="205"/>
+      <c r="I29" s="205"/>
+      <c r="J29" s="206"/>
     </row>
     <row r="30" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A30" s="117" t="s">
@@ -9404,16 +9411,16 @@
       </c>
     </row>
     <row r="32" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A32" s="214"/>
-      <c r="B32" s="215"/>
-      <c r="C32" s="215"/>
-      <c r="D32" s="215"/>
-      <c r="E32" s="215"/>
-      <c r="F32" s="215"/>
-      <c r="G32" s="215"/>
-      <c r="H32" s="215"/>
-      <c r="I32" s="215"/>
-      <c r="J32" s="216"/>
+      <c r="A32" s="204"/>
+      <c r="B32" s="205"/>
+      <c r="C32" s="205"/>
+      <c r="D32" s="205"/>
+      <c r="E32" s="205"/>
+      <c r="F32" s="205"/>
+      <c r="G32" s="205"/>
+      <c r="H32" s="205"/>
+      <c r="I32" s="205"/>
+      <c r="J32" s="206"/>
     </row>
     <row r="33" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A33" s="121" t="s">
@@ -9455,7 +9462,9 @@
       <c r="C34" s="122">
         <v>254</v>
       </c>
-      <c r="D34" s="122"/>
+      <c r="D34" s="122" t="s">
+        <v>419</v>
+      </c>
       <c r="E34" s="122"/>
       <c r="F34" s="122"/>
       <c r="G34" s="125"/>
@@ -9688,14 +9697,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="A29:J29"/>
-    <mergeCell ref="A32:J32"/>
-    <mergeCell ref="A4:A13"/>
-    <mergeCell ref="A14:J14"/>
-    <mergeCell ref="A17:J17"/>
-    <mergeCell ref="A20:J20"/>
-    <mergeCell ref="A23:J23"/>
-    <mergeCell ref="A26:J26"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="B2:B3"/>
@@ -9706,6 +9707,14 @@
     <mergeCell ref="H2:H3"/>
     <mergeCell ref="I2:I3"/>
     <mergeCell ref="J2:J3"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A32:J32"/>
+    <mergeCell ref="A4:A13"/>
+    <mergeCell ref="A14:J14"/>
+    <mergeCell ref="A17:J17"/>
+    <mergeCell ref="A20:J20"/>
+    <mergeCell ref="A23:J23"/>
+    <mergeCell ref="A26:J26"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>